<commit_message>
Excel and test updated
</commit_message>
<xml_diff>
--- a/Docs/DataRepo_UnitTestCases.xlsx
+++ b/Docs/DataRepo_UnitTestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work Jean\DotNet Modules\Data Repo\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23C89C3E-1B1A-4FC8-95FE-CB8AB05A60AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D715B94F-3B93-46C7-A668-5DA611FAF45A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="226">
   <si>
     <t>Test ID</t>
   </si>
@@ -218,18 +218,9 @@
     <t>Concurrent writes to different keys succeed</t>
   </si>
   <si>
-    <t>Concurrent writes to same key are consistent</t>
-  </si>
-  <si>
     <t>LastStructureChangeUtc updates on structural ops</t>
   </si>
   <si>
-    <t>Invalid JSON is rejected</t>
-  </si>
-  <si>
-    <t>Repository snapshot export is stable</t>
-  </si>
-  <si>
     <t>Key name case sensitivity</t>
   </si>
   <si>
@@ -242,9 +233,6 @@
     <t>Clear repository removes all keys</t>
   </si>
   <si>
-    <t>Load initial keys from definition</t>
-  </si>
-  <si>
     <t>IRepoConsumer receives change notifications</t>
   </si>
   <si>
@@ -326,24 +314,9 @@
     <t>Key 'unknown' does not exist</t>
   </si>
   <si>
-    <t>CreateKey("tempKey", Integer, deletePass="d123"); value set</t>
-  </si>
-  <si>
     <t>Keys k1..k100 exist (Integer)</t>
   </si>
   <si>
-    <t>Key 'counter' exists (Integer)</t>
-  </si>
-  <si>
-    <t>Record LastStructureChangeUtc=T0; ensure small wait</t>
-  </si>
-  <si>
-    <t>Key 'cfg' is JSON; typeEnforcement=true</t>
-  </si>
-  <si>
-    <t>Repo contains several keys/values</t>
-  </si>
-  <si>
     <t>Repository empty</t>
   </si>
   <si>
@@ -353,9 +326,6 @@
     <t>Repo contains keys</t>
   </si>
   <si>
-    <t>Have a definition list/dictionary</t>
-  </si>
-  <si>
     <t>Consumer subscribed to repo</t>
   </si>
   <si>
@@ -374,57 +344,12 @@
     <t>Instantiate DataRepo() with default parameters.</t>
   </si>
   <si>
-    <t>DeleteKey("tempKey") without password; then DeleteKey with deletePass="d123".</t>
-  </si>
-  <si>
-    <t>Call CreateKeyMulti with list: [('a', Integer), ('b', String), ('c', Bool)].</t>
-  </si>
-  <si>
     <t>Spawn N threads, each Write(k_i, i). Wait for all to complete.</t>
   </si>
   <si>
-    <t>Spawn N threads writing sequential integers; optionally use Interlocked for increments if supported.</t>
-  </si>
-  <si>
-    <t>CreateKey('new', String); capture T1; DeleteKey('new'); capture T2.</t>
-  </si>
-  <si>
-    <t>Write("cfg", "{bad json}").</t>
-  </si>
-  <si>
-    <t>Call ToString()/Export() method if available.</t>
-  </si>
-  <si>
-    <t>CreateKey("Mode", String); attempt Read("mode").</t>
-  </si>
-  <si>
-    <t>Write("mode", "manual"); Read("mode").</t>
-  </si>
-  <si>
-    <t>Write("mode", null) and Write("mode", "").</t>
-  </si>
-  <si>
-    <t>Call Clear().</t>
-  </si>
-  <si>
-    <t>Initialize DataRepo with initial map.</t>
-  </si>
-  <si>
     <t>Write to a key and observe callback/event.</t>
   </si>
   <si>
-    <t>Call WriteKeyMulti with: [('a',10), ('b','hello'), ('c',true)]</t>
-  </si>
-  <si>
-    <t>Call SetKeyNullMulti(['k1','k3'])</t>
-  </si>
-  <si>
-    <t>Call FindKeysWithWildcards('cfg.*'), then FindKeysWithWildcards('cfg.*.value'); also test empty filter error</t>
-  </si>
-  <si>
-    <t>Create keys for A1 and B2; call GetEntityIds('devices') and order ascending</t>
-  </si>
-  <si>
     <t>new DataRepo()</t>
   </si>
   <si>
@@ -458,39 +383,12 @@
     <t>Key='unknown'</t>
   </si>
   <si>
-    <t>3 keys</t>
-  </si>
-  <si>
     <t>Values 1..100</t>
   </si>
   <si>
-    <t>Sequence 1..N</t>
-  </si>
-  <si>
-    <t>"{bad json}"</t>
-  </si>
-  <si>
-    <t>"manual"</t>
-  </si>
-  <si>
-    <t>null / empty</t>
-  </si>
-  <si>
-    <t>Definition map</t>
-  </si>
-  <si>
     <t>Value change</t>
   </si>
   <si>
-    <t>WriteKeyMulti list and optional writePass</t>
-  </si>
-  <si>
-    <t>['k1','k3']</t>
-  </si>
-  <si>
-    <t>Patterns 'cfg.*' and 'cfg.*.value'</t>
-  </si>
-  <si>
     <t>Base='devices'</t>
   </si>
   <si>
@@ -530,51 +428,21 @@
     <t>First delete is rejected; second delete succeeds; Count decrements; LastStructureChangeUtc updated.</t>
   </si>
   <si>
-    <t>All keys created atomically or per-item; Count increases accordingly; LastStructureChangeUtc updated.</t>
-  </si>
-  <si>
     <t>All writes succeed; final values match; no data races/exceptions.</t>
   </si>
   <si>
-    <t>No corruption/exceptions; final value equals last successful write by happens-before order.</t>
-  </si>
-  <si>
     <t>T1 &gt; T0; T2 &gt; T1 (monotonic increase on create/delete).</t>
   </si>
   <si>
-    <t>Operation rejected with parse/type error; previous value unchanged.</t>
-  </si>
-  <si>
-    <t>Returns a deterministic snapshot representation without exposing secrets (passwords not included).</t>
-  </si>
-  <si>
-    <t>Define expected behavior: either keys are case-sensitive (not found) or case-insensitive (returns value).</t>
-  </si>
-  <si>
     <t>Read returns "manual"; no duplication.</t>
   </si>
   <si>
-    <t>Define behavior: null rejected or stored; empty allowed as empty string.</t>
-  </si>
-  <si>
-    <t>Count==0; LastStructureChangeUtc updated.</t>
-  </si>
-  <si>
     <t>All keys created with correct types and values.</t>
   </si>
   <si>
     <t>Consumer receives notification with correct key, old/new value.</t>
   </si>
   <si>
-    <t>Values set: Read('a')='10', Read('b')='hello', Read('c')='True'</t>
-  </si>
-  <si>
-    <t>ReadKeyString('k1')=='' and ReadKeyString('k3')==''; 'k2' unchanged</t>
-  </si>
-  <si>
-    <t>First call returns all under 'cfg.' including nested; second returns only 'cfg.detail.value'; empty filter throws ArgumentException</t>
-  </si>
-  <si>
     <t>Returned IDs == ['A1','B2']</t>
   </si>
   <si>
@@ -687,6 +555,150 @@
   </si>
   <si>
     <t>First read is rejected; second read returns "top".</t>
+  </si>
+  <si>
+    <t>CreateAndWriteKey("tempKey", Integer, value=7, deletePass="d123")</t>
+  </si>
+  <si>
+    <t>DeleteKey() without password, DeleteKey() with deletePass="d123".</t>
+  </si>
+  <si>
+    <t>deletePass='d123'</t>
+  </si>
+  <si>
+    <t>CreateKeyMulti()</t>
+  </si>
+  <si>
+    <t>list: [('a.x', Integer), ('a.y', String), ('a.z', Bool)]</t>
+  </si>
+  <si>
+    <t>All keys created; Count increases accordingly; LastStructureChangeUtc updated.</t>
+  </si>
+  <si>
+    <t>Set a null Key</t>
+  </si>
+  <si>
+    <t>SetKeyNull("mode")</t>
+  </si>
+  <si>
+    <t>Repository unchanged, keeping its values.</t>
+  </si>
+  <si>
+    <t>Record LastStructureChangeUtc=T0</t>
+  </si>
+  <si>
+    <t>CreateKey(), capture T1, DeleteKey(), capture T2</t>
+  </si>
+  <si>
+    <t>Key='new', Type=String</t>
+  </si>
+  <si>
+    <t>AppendKeyEntityId</t>
+  </si>
+  <si>
+    <t>Key='base', id='id', addDot='true'/false'</t>
+  </si>
+  <si>
+    <t>DataRepo.AppendKeyEntityId() with addDot true/with addDot false</t>
+  </si>
+  <si>
+    <t>First Call the result excpected is: "base.{id}."; Second: "base.{id}"</t>
+  </si>
+  <si>
+    <t>AppendKeyArrayIndex</t>
+  </si>
+  <si>
+    <t>DataRepo.AppendKeyArrayIndex() with addDot true/with addDot false</t>
+  </si>
+  <si>
+    <t>Key='base', idx=3/0, addDot='true'/false'</t>
+  </si>
+  <si>
+    <t>First Call the result excpected is: "base.[3]."; Second: "base.[0]"</t>
+  </si>
+  <si>
+    <t>CreateKey(), WriteKey(), ReadKey('mode')</t>
+  </si>
+  <si>
+    <t>Key='Mode', Type=String, Value=auto</t>
+  </si>
+  <si>
+    <t>Define expected behavior: either keys are case-sensitive (not found) or case-insensitive (returns value). ('Mode' != 'mode')</t>
+  </si>
+  <si>
+    <t>Value = "manual"</t>
+  </si>
+  <si>
+    <t>Key 'name' exists</t>
+  </si>
+  <si>
+    <t>Value = null / empty</t>
+  </si>
+  <si>
+    <t>WriteKey(), ReadKeyString(), WriteKey(), ReadKeyString()</t>
+  </si>
+  <si>
+    <t>Null stored as empty value; empty allowed as empty string.</t>
+  </si>
+  <si>
+    <t>DeleteKeysMulti(), GetAll()</t>
+  </si>
+  <si>
+    <t>Repository empty; Count==0; LastStructureChangeUtc updated.</t>
+  </si>
+  <si>
+    <t>Create from Json</t>
+  </si>
+  <si>
+    <t>CreateFromJson(),GetAll()</t>
+  </si>
+  <si>
+    <t>Json='\"cfg\": { \"a\": 1, \"b\": \"x\" }, \"enabled\": true'</t>
+  </si>
+  <si>
+    <t>valuesList: [('a',10), ('b','hello'), ('c',true)]</t>
+  </si>
+  <si>
+    <t>WriteKeyMulti(), ReadKeyString()</t>
+  </si>
+  <si>
+    <t>Batch write multiple keys with password</t>
+  </si>
+  <si>
+    <t>Keys 'p1' (Integer), 'p2' (Integer) with passWrite='w' exist</t>
+  </si>
+  <si>
+    <t>WriteKeyMulti() with writePass='bad'/WriteKeyMulti() with writePass='w', ReadKeyString()</t>
+  </si>
+  <si>
+    <t>Value = 1/2, writePass='bad'/'w'</t>
+  </si>
+  <si>
+    <t>First call UnauthorizedAccesException, Second: (p1) = 1, (p2) = 2.</t>
+  </si>
+  <si>
+    <t>Values set: Read('a')='10', Read('b')='hello', Read('c')='True'.</t>
+  </si>
+  <si>
+    <t>SetKeyNullMulti(['k1','k3'])</t>
+  </si>
+  <si>
+    <t>FindKeysWithWildcards()</t>
+  </si>
+  <si>
+    <t>Value='cfg.*' / 'cfg.*.value' / empty</t>
+  </si>
+  <si>
+    <t>First call returns all under 'cfg.' including nested; second returns only 'cfg.detail.value'; empty filter throws ArgumentException.</t>
+  </si>
+  <si>
+    <t>ReadKeyString('k1')=='' and ReadKeyString('k3')==''; 'k2' unchanged.</t>
+  </si>
+  <si>
+    <t>DR-035</t>
+  </si>
+  <si>
+    <t>Createkeys() for A1 and B2, GetEntityIds('devices') and order ascending</t>
   </si>
 </sst>
 </file>
@@ -717,14 +729,13 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -734,11 +745,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -781,22 +787,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="2" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+  <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1100,10 +1102,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L36"/>
+  <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1115,7 +1117,7 @@
     <col min="5" max="5" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="91.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="97.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="47.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="51.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="116.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="6.42578125" bestFit="1" customWidth="1"/>
@@ -1168,27 +1170,27 @@
         <v>46</v>
       </c>
       <c r="C2" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E2" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="F2" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="G2" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="H2" t="s">
-        <v>134</v>
+        <v>109</v>
       </c>
       <c r="I2" t="s">
-        <v>157</v>
-      </c>
-      <c r="J2" s="3"/>
+        <v>123</v>
+      </c>
+      <c r="J2" s="2"/>
     </row>
     <row r="3" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -1198,27 +1200,27 @@
         <v>47</v>
       </c>
       <c r="C3" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D3" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E3" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="F3" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="G3" t="s">
-        <v>201</v>
+        <v>157</v>
       </c>
       <c r="H3" t="s">
-        <v>135</v>
+        <v>110</v>
       </c>
       <c r="I3" t="s">
-        <v>158</v>
-      </c>
-      <c r="J3" s="3"/>
+        <v>124</v>
+      </c>
+      <c r="J3" s="2"/>
     </row>
     <row r="4" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -1228,27 +1230,27 @@
         <v>48</v>
       </c>
       <c r="C4" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D4" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E4" t="s">
+        <v>82</v>
+      </c>
+      <c r="F4" t="s">
         <v>86</v>
       </c>
-      <c r="F4" t="s">
-        <v>90</v>
-      </c>
       <c r="G4" t="s">
-        <v>202</v>
+        <v>158</v>
       </c>
       <c r="H4" t="s">
-        <v>136</v>
+        <v>111</v>
       </c>
       <c r="I4" t="s">
-        <v>206</v>
-      </c>
-      <c r="J4" s="3"/>
+        <v>162</v>
+      </c>
+      <c r="J4" s="2"/>
     </row>
     <row r="5" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -1258,27 +1260,27 @@
         <v>49</v>
       </c>
       <c r="C5" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D5" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E5" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="F5" t="s">
-        <v>195</v>
+        <v>151</v>
       </c>
       <c r="G5" t="s">
-        <v>203</v>
+        <v>159</v>
       </c>
       <c r="H5" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="I5" t="s">
-        <v>196</v>
-      </c>
-      <c r="J5" s="3"/>
+        <v>152</v>
+      </c>
+      <c r="J5" s="2"/>
     </row>
     <row r="6" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -1288,27 +1290,27 @@
         <v>50</v>
       </c>
       <c r="C6" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D6" t="s">
+        <v>78</v>
+      </c>
+      <c r="E6" t="s">
         <v>82</v>
       </c>
-      <c r="E6" t="s">
-        <v>86</v>
-      </c>
       <c r="F6" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="G6" t="s">
-        <v>202</v>
+        <v>158</v>
       </c>
       <c r="H6" t="s">
-        <v>197</v>
+        <v>153</v>
       </c>
       <c r="I6" t="s">
-        <v>159</v>
-      </c>
-      <c r="J6" s="3"/>
+        <v>125</v>
+      </c>
+      <c r="J6" s="2"/>
     </row>
     <row r="7" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -1318,29 +1320,29 @@
         <v>51</v>
       </c>
       <c r="C7" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D7" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E7" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F7" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="G7" t="s">
-        <v>202</v>
+        <v>158</v>
       </c>
       <c r="H7" t="s">
-        <v>198</v>
+        <v>154</v>
       </c>
       <c r="I7" t="s">
-        <v>160</v>
-      </c>
-      <c r="J7" s="3"/>
-    </row>
-    <row r="8" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+      <c r="J7" s="2"/>
+    </row>
+    <row r="8" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -1348,28 +1350,29 @@
         <v>52</v>
       </c>
       <c r="C8" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D8" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E8" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="F8" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="G8" t="s">
-        <v>201</v>
+        <v>157</v>
       </c>
       <c r="H8" t="s">
-        <v>137</v>
+        <v>112</v>
       </c>
       <c r="I8" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+      <c r="J8" s="2"/>
+    </row>
+    <row r="9" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -1377,28 +1380,29 @@
         <v>53</v>
       </c>
       <c r="C9" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D9" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E9" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="F9" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="G9" t="s">
-        <v>200</v>
+        <v>156</v>
       </c>
       <c r="H9" t="s">
-        <v>138</v>
+        <v>113</v>
       </c>
       <c r="I9" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+      <c r="J9" s="2"/>
+    </row>
+    <row r="10" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -1406,28 +1410,29 @@
         <v>54</v>
       </c>
       <c r="C10" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D10" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E10" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="F10" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="G10" t="s">
-        <v>199</v>
+        <v>155</v>
       </c>
       <c r="H10" t="s">
-        <v>139</v>
+        <v>114</v>
       </c>
       <c r="I10" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+      <c r="J10" s="2"/>
+    </row>
+    <row r="11" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -1435,28 +1440,29 @@
         <v>55</v>
       </c>
       <c r="C11" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D11" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E11" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F11" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="G11" t="s">
-        <v>204</v>
+        <v>160</v>
       </c>
       <c r="H11" t="s">
-        <v>140</v>
+        <v>115</v>
       </c>
       <c r="I11" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+      <c r="J11" s="2"/>
+    </row>
+    <row r="12" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -1464,29 +1470,29 @@
         <v>56</v>
       </c>
       <c r="C12" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D12" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E12" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F12" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="G12" t="s">
-        <v>207</v>
+        <v>163</v>
       </c>
       <c r="H12" t="s">
-        <v>141</v>
+        <v>116</v>
       </c>
       <c r="I12" t="s">
-        <v>164</v>
+        <v>130</v>
       </c>
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -1494,56 +1500,57 @@
         <v>57</v>
       </c>
       <c r="C13" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D13" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E13" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F13" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="G13" t="s">
-        <v>207</v>
+        <v>163</v>
       </c>
       <c r="H13" t="s">
-        <v>142</v>
+        <v>117</v>
       </c>
       <c r="I13" t="s">
-        <v>208</v>
-      </c>
+        <v>164</v>
+      </c>
+      <c r="J13" s="2"/>
     </row>
     <row r="14" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>24</v>
       </c>
       <c r="B14" t="s">
-        <v>209</v>
+        <v>165</v>
       </c>
       <c r="C14" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D14" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E14" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="F14" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="G14" t="s">
-        <v>211</v>
+        <v>167</v>
       </c>
       <c r="H14" t="s">
-        <v>210</v>
+        <v>166</v>
       </c>
       <c r="I14" t="s">
-        <v>165</v>
-      </c>
-      <c r="J14" s="3"/>
+        <v>131</v>
+      </c>
+      <c r="J14" s="2"/>
     </row>
     <row r="15" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -1553,27 +1560,27 @@
         <v>58</v>
       </c>
       <c r="C15" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D15" t="s">
+        <v>78</v>
+      </c>
+      <c r="E15" t="s">
         <v>82</v>
       </c>
-      <c r="E15" t="s">
-        <v>86</v>
-      </c>
       <c r="F15" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="G15" t="s">
-        <v>212</v>
+        <v>168</v>
       </c>
       <c r="H15" t="s">
-        <v>143</v>
+        <v>118</v>
       </c>
       <c r="I15" t="s">
-        <v>213</v>
-      </c>
-      <c r="J15" s="3"/>
+        <v>169</v>
+      </c>
+      <c r="J15" s="2"/>
     </row>
     <row r="16" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
@@ -1583,27 +1590,27 @@
         <v>59</v>
       </c>
       <c r="C16" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D16" t="s">
+        <v>78</v>
+      </c>
+      <c r="E16" t="s">
         <v>82</v>
       </c>
-      <c r="E16" t="s">
-        <v>86</v>
-      </c>
       <c r="F16" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="G16" t="s">
-        <v>214</v>
+        <v>170</v>
       </c>
       <c r="H16" t="s">
-        <v>144</v>
+        <v>119</v>
       </c>
       <c r="I16" t="s">
-        <v>166</v>
-      </c>
-      <c r="J16" s="3"/>
+        <v>132</v>
+      </c>
+      <c r="J16" s="2"/>
     </row>
     <row r="17" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
@@ -1613,27 +1620,27 @@
         <v>60</v>
       </c>
       <c r="C17" t="s">
+        <v>75</v>
+      </c>
+      <c r="D17" t="s">
         <v>79</v>
       </c>
-      <c r="D17" t="s">
-        <v>83</v>
-      </c>
       <c r="E17" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="F17" t="s">
-        <v>215</v>
+        <v>171</v>
       </c>
       <c r="G17" t="s">
-        <v>217</v>
+        <v>173</v>
       </c>
       <c r="H17" t="s">
-        <v>216</v>
+        <v>172</v>
       </c>
       <c r="I17" t="s">
-        <v>167</v>
-      </c>
-      <c r="J17" s="3"/>
+        <v>133</v>
+      </c>
+      <c r="J17" s="2"/>
     </row>
     <row r="18" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
@@ -1643,27 +1650,27 @@
         <v>61</v>
       </c>
       <c r="C18" t="s">
+        <v>75</v>
+      </c>
+      <c r="D18" t="s">
         <v>79</v>
       </c>
-      <c r="D18" t="s">
-        <v>83</v>
-      </c>
       <c r="E18" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="F18" t="s">
-        <v>218</v>
+        <v>174</v>
       </c>
       <c r="G18" t="s">
-        <v>219</v>
+        <v>175</v>
       </c>
       <c r="H18" t="s">
-        <v>220</v>
+        <v>176</v>
       </c>
       <c r="I18" t="s">
-        <v>221</v>
-      </c>
-      <c r="J18" s="3"/>
+        <v>177</v>
+      </c>
+      <c r="J18" s="2"/>
     </row>
     <row r="19" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
@@ -1673,24 +1680,27 @@
         <v>62</v>
       </c>
       <c r="C19" t="s">
+        <v>75</v>
+      </c>
+      <c r="D19" t="s">
         <v>79</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>83</v>
       </c>
-      <c r="E19" t="s">
-        <v>87</v>
-      </c>
       <c r="F19" t="s">
-        <v>101</v>
+        <v>178</v>
       </c>
       <c r="G19" t="s">
-        <v>117</v>
+        <v>179</v>
+      </c>
+      <c r="H19" t="s">
+        <v>180</v>
       </c>
       <c r="I19" t="s">
-        <v>168</v>
-      </c>
-      <c r="J19" s="4"/>
+        <v>134</v>
+      </c>
+      <c r="J19" s="2"/>
     </row>
     <row r="20" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
@@ -1700,27 +1710,27 @@
         <v>63</v>
       </c>
       <c r="C20" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D20" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E20" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F20" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="G20" t="s">
-        <v>118</v>
+        <v>181</v>
       </c>
       <c r="H20" t="s">
-        <v>145</v>
+        <v>182</v>
       </c>
       <c r="I20" t="s">
-        <v>169</v>
-      </c>
-      <c r="J20" s="4"/>
+        <v>183</v>
+      </c>
+      <c r="J20" s="2"/>
     </row>
     <row r="21" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
@@ -1730,438 +1740,480 @@
         <v>64</v>
       </c>
       <c r="C21" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D21" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E21" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="F21" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="G21" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="H21" t="s">
-        <v>146</v>
+        <v>120</v>
       </c>
       <c r="I21" t="s">
-        <v>170</v>
-      </c>
-      <c r="J21" s="4"/>
+        <v>135</v>
+      </c>
     </row>
     <row r="22" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>32</v>
       </c>
       <c r="B22" t="s">
-        <v>65</v>
+        <v>184</v>
       </c>
       <c r="C22" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D22" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E22" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F22" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="G22" t="s">
-        <v>120</v>
+        <v>185</v>
       </c>
       <c r="H22" t="s">
-        <v>147</v>
+        <v>85</v>
       </c>
       <c r="I22" t="s">
-        <v>171</v>
-      </c>
-      <c r="J22" s="4"/>
+        <v>186</v>
+      </c>
+      <c r="J22" s="2"/>
     </row>
     <row r="23" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>33</v>
       </c>
       <c r="B23" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C23" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D23" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E23" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F23" t="s">
-        <v>104</v>
+        <v>187</v>
       </c>
       <c r="G23" t="s">
-        <v>121</v>
+        <v>188</v>
+      </c>
+      <c r="H23" t="s">
+        <v>189</v>
       </c>
       <c r="I23" t="s">
-        <v>172</v>
-      </c>
-      <c r="J23" s="4"/>
+        <v>136</v>
+      </c>
+      <c r="J23" s="2"/>
     </row>
     <row r="24" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>34</v>
       </c>
       <c r="B24" t="s">
-        <v>67</v>
+        <v>190</v>
       </c>
       <c r="C24" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D24" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E24" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="F24" t="s">
-        <v>105</v>
+        <v>85</v>
       </c>
       <c r="G24" t="s">
-        <v>122</v>
+        <v>192</v>
       </c>
       <c r="H24" t="s">
-        <v>148</v>
+        <v>191</v>
       </c>
       <c r="I24" t="s">
-        <v>173</v>
-      </c>
-      <c r="J24" s="4"/>
+        <v>193</v>
+      </c>
+      <c r="J24" s="2"/>
     </row>
     <row r="25" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>35</v>
       </c>
       <c r="B25" t="s">
-        <v>68</v>
+        <v>194</v>
       </c>
       <c r="C25" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D25" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E25" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="F25" t="s">
-        <v>106</v>
+        <v>85</v>
       </c>
       <c r="G25" t="s">
-        <v>123</v>
+        <v>195</v>
+      </c>
+      <c r="H25" t="s">
+        <v>196</v>
       </c>
       <c r="I25" t="s">
-        <v>174</v>
-      </c>
-      <c r="J25" s="4"/>
+        <v>197</v>
+      </c>
+      <c r="J25" s="2"/>
     </row>
     <row r="26" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>36</v>
       </c>
       <c r="B26" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C26" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D26" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E26" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="F26" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="G26" t="s">
-        <v>124</v>
+        <v>198</v>
+      </c>
+      <c r="H26" t="s">
+        <v>199</v>
       </c>
       <c r="I26" t="s">
-        <v>175</v>
-      </c>
-      <c r="J26" s="4"/>
+        <v>200</v>
+      </c>
+      <c r="J26" s="2"/>
     </row>
     <row r="27" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>37</v>
       </c>
       <c r="B27" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C27" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D27" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E27" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F27" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="G27" t="s">
-        <v>125</v>
+        <v>156</v>
       </c>
       <c r="H27" t="s">
-        <v>149</v>
+        <v>201</v>
       </c>
       <c r="I27" t="s">
-        <v>176</v>
-      </c>
-      <c r="J27" s="4"/>
+        <v>137</v>
+      </c>
+      <c r="J27" s="2"/>
     </row>
     <row r="28" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>38</v>
       </c>
       <c r="B28" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C28" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D28" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E28" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F28" t="s">
-        <v>94</v>
+        <v>202</v>
       </c>
       <c r="G28" t="s">
-        <v>126</v>
+        <v>204</v>
       </c>
       <c r="H28" t="s">
-        <v>150</v>
+        <v>203</v>
       </c>
       <c r="I28" t="s">
-        <v>177</v>
-      </c>
-      <c r="J28" s="4"/>
+        <v>205</v>
+      </c>
+      <c r="J28" s="2"/>
     </row>
     <row r="29" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>39</v>
       </c>
       <c r="B29" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C29" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D29" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E29" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="F29" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="G29" t="s">
-        <v>127</v>
+        <v>206</v>
+      </c>
+      <c r="H29" t="s">
+        <v>85</v>
       </c>
       <c r="I29" t="s">
-        <v>178</v>
-      </c>
-      <c r="J29" s="4"/>
+        <v>207</v>
+      </c>
+      <c r="J29" s="2"/>
     </row>
     <row r="30" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>40</v>
       </c>
       <c r="B30" t="s">
-        <v>73</v>
+        <v>208</v>
       </c>
       <c r="C30" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D30" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E30" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="F30" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="G30" t="s">
-        <v>128</v>
+        <v>209</v>
       </c>
       <c r="H30" t="s">
-        <v>151</v>
+        <v>210</v>
       </c>
       <c r="I30" t="s">
-        <v>179</v>
-      </c>
-      <c r="J30" s="4"/>
+        <v>138</v>
+      </c>
+      <c r="J30" s="2"/>
     </row>
     <row r="31" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>41</v>
       </c>
       <c r="B31" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C31" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D31" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E31" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F31" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="G31" t="s">
-        <v>129</v>
+        <v>108</v>
       </c>
       <c r="H31" t="s">
-        <v>152</v>
+        <v>121</v>
       </c>
       <c r="I31" t="s">
-        <v>180</v>
-      </c>
-      <c r="J31" s="4"/>
+        <v>139</v>
+      </c>
+      <c r="J31" s="2"/>
     </row>
     <row r="32" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>42</v>
       </c>
       <c r="B32" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C32" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D32" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E32" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="F32" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="G32" t="s">
-        <v>130</v>
+        <v>212</v>
       </c>
       <c r="H32" t="s">
-        <v>153</v>
+        <v>211</v>
       </c>
       <c r="I32" t="s">
-        <v>181</v>
-      </c>
-      <c r="J32" s="4"/>
+        <v>218</v>
+      </c>
+      <c r="J32" s="2"/>
     </row>
     <row r="33" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>43</v>
       </c>
       <c r="B33" t="s">
-        <v>76</v>
+        <v>213</v>
       </c>
       <c r="C33" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D33" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E33" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F33" t="s">
-        <v>113</v>
+        <v>214</v>
       </c>
       <c r="G33" t="s">
-        <v>131</v>
+        <v>215</v>
       </c>
       <c r="H33" t="s">
-        <v>154</v>
+        <v>216</v>
       </c>
       <c r="I33" t="s">
-        <v>182</v>
-      </c>
-      <c r="J33" s="4"/>
+        <v>217</v>
+      </c>
+      <c r="J33" s="2"/>
     </row>
     <row r="34" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>44</v>
       </c>
       <c r="B34" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C34" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D34" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E34" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F34" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="G34" t="s">
-        <v>132</v>
+        <v>219</v>
       </c>
       <c r="H34" t="s">
-        <v>155</v>
+        <v>85</v>
       </c>
       <c r="I34" t="s">
-        <v>183</v>
-      </c>
-      <c r="J34" s="4"/>
+        <v>223</v>
+      </c>
+      <c r="J34" s="2"/>
     </row>
     <row r="35" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>45</v>
       </c>
       <c r="B35" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C35" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D35" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E35" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F35" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="G35" t="s">
-        <v>133</v>
+        <v>220</v>
       </c>
       <c r="H35" t="s">
-        <v>156</v>
+        <v>221</v>
       </c>
       <c r="I35" t="s">
-        <v>184</v>
-      </c>
-      <c r="J35" s="4"/>
-    </row>
-    <row r="36" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+        <v>222</v>
+      </c>
+      <c r="J35" s="2"/>
+    </row>
+    <row r="36" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>224</v>
+      </c>
+      <c r="B36" t="s">
+        <v>74</v>
+      </c>
+      <c r="C36" t="s">
+        <v>75</v>
+      </c>
+      <c r="D36" t="s">
+        <v>77</v>
+      </c>
+      <c r="E36" t="s">
+        <v>83</v>
+      </c>
+      <c r="F36" t="s">
+        <v>105</v>
+      </c>
+      <c r="G36" t="s">
+        <v>225</v>
+      </c>
+      <c r="H36" t="s">
+        <v>122</v>
+      </c>
+      <c r="I36" t="s">
+        <v>140</v>
+      </c>
+      <c r="J36" s="2"/>
+    </row>
+    <row r="37" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2176,42 +2228,42 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>185</v>
+        <v>141</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>186</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>187</v>
+        <v>143</v>
       </c>
       <c r="B2" t="s">
-        <v>191</v>
+        <v>147</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>188</v>
+        <v>144</v>
       </c>
       <c r="B3" t="s">
-        <v>192</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>189</v>
+        <v>145</v>
       </c>
       <c r="B4" t="s">
-        <v>193</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>190</v>
+        <v>146</v>
       </c>
       <c r="B5" t="s">
-        <v>194</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>